<commit_message>
ADded flask SQL Alchemy trick
</commit_message>
<xml_diff>
--- a/Elegant_Python.xlsx
+++ b/Elegant_Python.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="879" firstSheet="3" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="879" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flask" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="1022">
   <si>
     <r>
       <rPr>
@@ -21478,6 +21478,460 @@
   <si>
     <t>Таблица "Users" в формате класса Алхимии
 # relationship - не фактическое поле, а высокоуровновая ссылка для отношения между объектами ORM</t>
+  </si>
+  <si>
+    <t>Удалить старый Primary_key, создать новый, комплексный</t>
+  </si>
+  <si>
+    <r>
+      <t>def upgrade():
+    op.add_column(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'allowable_values'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, sa.Column(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'compressor_unit'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, sa.Text(), autoincrement=False, nullable=False), schema='vostok')
+    op.drop_constraint(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'allowable_values_pkey'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'allowable_values'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>type_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'primary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">', </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>schema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'vostok'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)
+    op.create_primary_key(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"allowable_values_pkey"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"allowable_values"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"tag_name", "compressor_unit"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>schema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'vostok'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)
+def downgrade():
+    op.create_primary_key(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"allowable_values_pkey"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> "allowable_values"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"tag_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, ], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>schema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'vostok'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)
+    op.drop_column(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'allowable_values'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'compressor_unit'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>schema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>'vostok'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -25113,8 +25567,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A52" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -26619,8 +27073,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -26936,9 +27390,13 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
+    <row r="49" spans="1:2" ht="145">
+      <c r="A49" s="11" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="20"/>
@@ -27023,7 +27481,7 @@
     <hyperlink ref="A29" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>

</xml_diff>

<commit_message>
Upd. Added rename column and JOin through merge in Pandas
</commit_message>
<xml_diff>
--- a/Elegant_Python.xlsx
+++ b/Elegant_Python.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="879" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="879" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Flask" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="1061">
   <si>
     <r>
       <rPr>
@@ -23811,7 +23811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -24186,23 +24186,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -24222,6 +24207,24 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -25951,59 +25954,59 @@
       <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A27" s="132" t="s">
+      <c r="A27" s="140" t="s">
         <v>893</v>
       </c>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
     </row>
     <row r="28" spans="1:7" ht="42.75" customHeight="1">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="139" t="s">
         <v>894</v>
       </c>
-      <c r="B28" s="131"/>
-      <c r="C28" s="131"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
       <c r="D28" s="27"/>
     </row>
     <row r="29" spans="1:7" ht="42.75" customHeight="1">
-      <c r="A29" s="131" t="s">
+      <c r="A29" s="139" t="s">
         <v>895</v>
       </c>
-      <c r="B29" s="131"/>
-      <c r="C29" s="131"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
       <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A30" s="131" t="s">
+      <c r="A30" s="139" t="s">
         <v>896</v>
       </c>
-      <c r="B30" s="131"/>
-      <c r="C30" s="131"/>
+      <c r="B30" s="139"/>
+      <c r="C30" s="139"/>
       <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:7" ht="33" customHeight="1">
-      <c r="A31" s="131" t="s">
+      <c r="A31" s="139" t="s">
         <v>897</v>
       </c>
-      <c r="B31" s="131"/>
-      <c r="C31" s="131"/>
+      <c r="B31" s="139"/>
+      <c r="C31" s="139"/>
       <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A32" s="131" t="s">
+      <c r="A32" s="139" t="s">
         <v>898</v>
       </c>
-      <c r="B32" s="131"/>
-      <c r="C32" s="131"/>
+      <c r="B32" s="139"/>
+      <c r="C32" s="139"/>
       <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1">
-      <c r="A33" s="131" t="s">
+      <c r="A33" s="139" t="s">
         <v>899</v>
       </c>
-      <c r="B33" s="131"/>
-      <c r="C33" s="131"/>
+      <c r="B33" s="139"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="27"/>
     </row>
   </sheetData>
@@ -26026,10 +26029,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
@@ -26088,204 +26091,228 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
     </row>
     <row r="9" spans="1:2" ht="29">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="110" t="s">
+        <v>982</v>
+      </c>
+      <c r="B9" s="110" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="24" t="s">
+        <v>985</v>
+      </c>
+      <c r="B10" s="130" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="24" t="s">
+        <v>986</v>
+      </c>
+      <c r="B11" s="130" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29">
+      <c r="A12" s="57" t="s">
         <v>334</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B12" s="57" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.5">
-      <c r="A10" s="54" t="s">
+    <row r="13" spans="1:2" ht="72.5">
+      <c r="A13" s="54" t="s">
         <v>1009</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B13" s="54" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="87">
-      <c r="A11" s="27" t="s">
+    <row r="14" spans="1:2" ht="87">
+      <c r="A14" s="27" t="s">
         <v>1008</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B14" s="54" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="87">
-      <c r="A12" s="24" t="s">
+    <row r="15" spans="1:2" ht="87">
+      <c r="A15" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B15" s="54" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="54"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="23" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="54"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B17" s="57" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="101.5">
-      <c r="A15" s="27" t="s">
+    <row r="18" spans="1:2" ht="101.5">
+      <c r="A18" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="B15" s="54"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="27"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
+      <c r="B18" s="54"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="27"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="B18" s="34"/>
-    </row>
-    <row r="19" spans="1:2" ht="58">
-      <c r="A19" s="27" t="s">
+      <c r="B21" s="34"/>
+    </row>
+    <row r="22" spans="1:2" ht="58">
+      <c r="A22" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B22" s="27" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="27"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="23" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="27"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B25" s="34" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="27" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B26" s="27" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="27" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B27" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="27"/>
-    </row>
-    <row r="27" spans="1:2" ht="29">
-      <c r="A27" s="23" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="27"/>
+    </row>
+    <row r="30" spans="1:2" ht="29">
+      <c r="A30" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B30" s="34" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="29">
-      <c r="A28" s="58" t="s">
+    <row r="31" spans="1:2" ht="29">
+      <c r="A31" s="58" t="s">
         <v>352</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B31" s="27" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="124"/>
-      <c r="B30" s="110"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-    </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="24"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="27"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="122"/>
-      <c r="B33" s="122"/>
+      <c r="A33" s="124"/>
+      <c r="B33" s="110"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="122"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="122"/>
-      <c r="B35" s="122"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="27"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="24"/>
+      <c r="A36" s="122"/>
       <c r="B36" s="122"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="122"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="122"/>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="24"/>
+      <c r="A38" s="122"/>
       <c r="B38" s="122"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="122"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="24"/>
+      <c r="A40" s="122"/>
       <c r="B40" s="122"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="122"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="122"/>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="24"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="122"/>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="122"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="122"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="24"/>
+      <c r="A44" s="122"/>
       <c r="B44" s="122"/>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="122"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="122"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="122"/>
+      <c r="B46" s="122"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="24"/>
+      <c r="B47" s="122"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="122"/>
+      <c r="B48" s="122"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -27123,8 +27150,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ158"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A133" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B139" sqref="A137:B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -27143,10 +27170,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="32" customFormat="1">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="142" t="s">
         <v>503</v>
       </c>
-      <c r="B2" s="135"/>
+      <c r="B2" s="143"/>
     </row>
     <row r="3" spans="1:2" s="71" customFormat="1">
       <c r="A3" s="24" t="s">
@@ -27445,10 +27472,10 @@
       <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:2" s="71" customFormat="1">
-      <c r="A44" s="134" t="s">
+      <c r="A44" s="142" t="s">
         <v>550</v>
       </c>
-      <c r="B44" s="135"/>
+      <c r="B44" s="143"/>
     </row>
     <row r="45" spans="1:2" s="71" customFormat="1" ht="58">
       <c r="A45" s="73" t="s">
@@ -27836,7 +27863,7 @@
       <c r="A102" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="B102" s="133" t="s">
+      <c r="B102" s="141" t="s">
         <v>641</v>
       </c>
     </row>
@@ -27844,7 +27871,7 @@
       <c r="A103" s="27" t="s">
         <v>642</v>
       </c>
-      <c r="B103" s="133"/>
+      <c r="B103" s="141"/>
     </row>
     <row r="104" spans="1:2" ht="43.5">
       <c r="A104" s="27" t="s">
@@ -29202,7 +29229,7 @@
       <c r="A18" s="27" t="s">
         <v>746</v>
       </c>
-      <c r="B18" s="133" t="s">
+      <c r="B18" s="141" t="s">
         <v>747</v>
       </c>
     </row>
@@ -29210,37 +29237,37 @@
       <c r="A19" s="83" t="s">
         <v>748</v>
       </c>
-      <c r="B19" s="133"/>
+      <c r="B19" s="141"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="83" t="s">
         <v>749</v>
       </c>
-      <c r="B20" s="133"/>
+      <c r="B20" s="141"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="83" t="s">
         <v>750</v>
       </c>
-      <c r="B21" s="133"/>
+      <c r="B21" s="141"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="83" t="s">
         <v>751</v>
       </c>
-      <c r="B22" s="133"/>
+      <c r="B22" s="141"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="83" t="s">
         <v>752</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="141"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="83" t="s">
         <v>753</v>
       </c>
-      <c r="B24" s="133"/>
+      <c r="B24" s="141"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="27"/>
@@ -30394,13 +30421,13 @@
       <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="136" t="s">
+      <c r="A20" s="131" t="s">
         <v>1047</v>
       </c>
-      <c r="B20" s="136"/>
+      <c r="B20" s="131"/>
     </row>
     <row r="21" spans="1:2" ht="116">
-      <c r="A21" s="137" t="s">
+      <c r="A21" s="132" t="s">
         <v>1048</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -30813,7 +30840,7 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -30823,34 +30850,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="133" t="s">
         <v>1052</v>
       </c>
-      <c r="B1" s="138"/>
+      <c r="B1" s="133"/>
     </row>
     <row r="2" spans="1:2" ht="29">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="134" t="s">
         <v>1059</v>
       </c>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="134" t="s">
         <v>1056</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="134" t="s">
         <v>1058</v>
       </c>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="134" t="s">
         <v>1057</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="55"/>
-      <c r="B4" s="139"/>
+      <c r="B4" s="134"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="139"/>
-      <c r="B5" s="139"/>
+      <c r="A5" s="134"/>
+      <c r="B5" s="134"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="45"/>
@@ -30869,14 +30896,14 @@
       <c r="B9" s="45"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="138" t="s">
+      <c r="A10" s="133" t="s">
         <v>1050</v>
       </c>
-      <c r="B10" s="138"/>
+      <c r="B10" s="133"/>
     </row>
     <row r="12" spans="1:2" ht="29">
       <c r="A12" s="45"/>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="135" t="s">
         <v>1054</v>
       </c>
     </row>
@@ -30891,16 +30918,16 @@
       <c r="B14" s="45"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="141" t="s">
+      <c r="A15" s="136" t="s">
         <v>1055</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="136"/>
     </row>
     <row r="16" spans="1:2" ht="58">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="137" t="s">
         <v>1060</v>
       </c>
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="134" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -31483,10 +31510,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="130" t="s">
+      <c r="A20" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="130"/>
+      <c r="B20" s="138"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="24" t="s">

</xml_diff>